<commit_message>
figuras actualizadas y correcciones menores
</commit_message>
<xml_diff>
--- a/tablas_agrupaciones_geográficas.xlsx
+++ b/tablas_agrupaciones_geográficas.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6a93ec0cea845852/2024-CMM_salud_digital/Proyecto_FONDEF_IRA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6a93ec0cea845852/2024-CMM_salud_digital/Proyecto_FONDEF_IRA/CMM-SD_comparacion_poblaciones_IRA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE25098D-3118-40A4-914E-CEB32E4EB057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="8_{AE25098D-3118-40A4-914E-CEB32E4EB057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{505C71EB-B2A0-4433-9C4D-74DACE4A9474}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="18192" windowHeight="11472" xr2:uid="{D77745BA-A4A0-43F6-BAC4-E2761BAEEF07}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="18192" windowHeight="11472" activeTab="2" xr2:uid="{D77745BA-A4A0-43F6-BAC4-E2761BAEEF07}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="39">
   <si>
     <t xml:space="preserve"> (0, 1)</t>
   </si>
@@ -139,6 +140,21 @@
   </si>
   <si>
     <t>(0,)</t>
+  </si>
+  <si>
+    <t>Menores_1</t>
+  </si>
+  <si>
+    <t>De_1_a_4</t>
+  </si>
+  <si>
+    <t>De_5_a_14</t>
+  </si>
+  <si>
+    <t>De_15_a_64</t>
+  </si>
+  <si>
+    <t>De_65_y_mas</t>
   </si>
 </sst>
 </file>
@@ -146,7 +162,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.00000"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -165,7 +181,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -269,24 +285,102 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -623,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84C03B65-580F-4B54-80A9-F65FA56D62F1}">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A41" sqref="A29:H41"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H4" sqref="G2:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1823,4 +1917,202 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABA08732-075E-494B-93A1-2378C1AEA10D}">
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="A1:F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="11.734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="8"/>
+      <c r="B1" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="11"/>
+      <c r="H1" s="13"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="18">
+        <v>0.69438800000000001</v>
+      </c>
+      <c r="C2" s="14">
+        <v>0.59142099999999997</v>
+      </c>
+      <c r="D2" s="14">
+        <v>0.60336599999999996</v>
+      </c>
+      <c r="E2" s="14">
+        <v>0.60043599999999997</v>
+      </c>
+      <c r="F2" s="15">
+        <v>0.65522899999999995</v>
+      </c>
+      <c r="G2" s="11"/>
+      <c r="H2" s="13"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="18">
+        <v>0.59142099999999997</v>
+      </c>
+      <c r="C3" s="14">
+        <v>0.73553299999999999</v>
+      </c>
+      <c r="D3" s="14">
+        <v>0.86971200000000004</v>
+      </c>
+      <c r="E3" s="14">
+        <v>0.54125000000000001</v>
+      </c>
+      <c r="F3" s="15">
+        <v>0.53515000000000001</v>
+      </c>
+      <c r="G3" s="11"/>
+      <c r="H3" s="13"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="18">
+        <v>0.60336599999999996</v>
+      </c>
+      <c r="C4" s="14">
+        <v>0.86971200000000004</v>
+      </c>
+      <c r="D4" s="14">
+        <v>0.81716599999999995</v>
+      </c>
+      <c r="E4" s="14">
+        <v>0.53635500000000003</v>
+      </c>
+      <c r="F4" s="15">
+        <v>0.58135300000000001</v>
+      </c>
+      <c r="G4" s="11"/>
+      <c r="H4" s="13"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="18">
+        <v>0.60043599999999997</v>
+      </c>
+      <c r="C5" s="14">
+        <v>0.54125000000000001</v>
+      </c>
+      <c r="D5" s="14">
+        <v>0.53635500000000003</v>
+      </c>
+      <c r="E5" s="14">
+        <v>0.72373600000000005</v>
+      </c>
+      <c r="F5" s="15">
+        <v>0.82210700000000003</v>
+      </c>
+      <c r="G5" s="11"/>
+      <c r="H5" s="13"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="19">
+        <v>0.65522899999999995</v>
+      </c>
+      <c r="C6" s="16">
+        <v>0.53515000000000001</v>
+      </c>
+      <c r="D6" s="16">
+        <v>0.58135300000000001</v>
+      </c>
+      <c r="E6" s="16">
+        <v>0.82210700000000003</v>
+      </c>
+      <c r="F6" s="17">
+        <v>0.84008799999999995</v>
+      </c>
+      <c r="G6" s="11"/>
+      <c r="H6" s="13"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="11"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="13"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="13"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="13"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="13"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>